<commit_message>
lla funciona la lectura y la tabla a la vez
</commit_message>
<xml_diff>
--- a/ej.xlsx
+++ b/ej.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\proyectos del cuarto semestre\analizadorDeDatos_Estadistica\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB577100-4E01-4C97-87C4-134A5E788A0A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C2B26CB-48AE-4380-AB56-E63E30584DC1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="696" yWindow="3312" windowWidth="17280" windowHeight="8880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="11424" yWindow="0" windowWidth="11712" windowHeight="12336" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -192,7 +192,7 @@
     <numFmt numFmtId="164" formatCode="#,##0%"/>
     <numFmt numFmtId="165" formatCode="#,##0.0"/>
   </numFmts>
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -232,6 +232,13 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="4">
@@ -404,7 +411,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="50">
+  <cellXfs count="51">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="4" fontId="2" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -498,6 +505,9 @@
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="4" fontId="3" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="3" fontId="3" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="3" fontId="4" fillId="2" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -540,9 +550,9 @@
     <xf numFmtId="3" fontId="1" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="4" fontId="3" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="165" fontId="3" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="3" fontId="3" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="3" fontId="6" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -850,8 +860,8 @@
   </sheetPr>
   <dimension ref="A1:S53"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:E1"/>
+    <sheetView tabSelected="1" topLeftCell="C10" workbookViewId="0">
+      <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -867,13 +877,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:19" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="47">
+      <c r="A1" s="33">
         <v>70</v>
       </c>
-      <c r="B1" s="48"/>
-      <c r="C1" s="49"/>
-      <c r="D1" s="49"/>
-      <c r="E1" s="47"/>
+      <c r="B1" s="34"/>
+      <c r="C1" s="35"/>
+      <c r="D1" s="35"/>
+      <c r="E1" s="33"/>
       <c r="F1" s="2"/>
       <c r="G1" s="8"/>
       <c r="H1" s="2"/>
@@ -888,7 +898,7 @@
     </row>
     <row r="2" spans="1:19" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="24">
-        <v>11111</v>
+        <v>11</v>
       </c>
       <c r="B2" s="25">
         <v>9</v>
@@ -1052,7 +1062,7 @@
       </c>
       <c r="J6" s="23">
         <f>MAX(A2:G11)</f>
-        <v>11111</v>
+        <v>11</v>
       </c>
       <c r="K6" s="1"/>
       <c r="M6" s="2"/>
@@ -1222,7 +1232,7 @@
       <c r="S11" s="2"/>
     </row>
     <row r="12" spans="1:19" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="26"/>
+      <c r="A12" s="50"/>
       <c r="B12" s="27"/>
       <c r="C12" s="2"/>
       <c r="D12" s="2"/>
@@ -1240,19 +1250,19 @@
       <c r="S12" s="2"/>
     </row>
     <row r="13" spans="1:19" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A13" s="33" t="s">
+      <c r="A13" s="36" t="s">
         <v>34</v>
       </c>
-      <c r="B13" s="34"/>
-      <c r="C13" s="33"/>
-      <c r="D13" s="33"/>
-      <c r="E13" s="35"/>
-      <c r="F13" s="33"/>
-      <c r="G13" s="36"/>
-      <c r="H13" s="33"/>
-      <c r="I13" s="35"/>
-      <c r="J13" s="35"/>
-      <c r="K13" s="35"/>
+      <c r="B13" s="37"/>
+      <c r="C13" s="36"/>
+      <c r="D13" s="36"/>
+      <c r="E13" s="38"/>
+      <c r="F13" s="36"/>
+      <c r="G13" s="39"/>
+      <c r="H13" s="36"/>
+      <c r="I13" s="38"/>
+      <c r="J13" s="38"/>
+      <c r="K13" s="38"/>
       <c r="M13" s="2"/>
       <c r="P13" s="1"/>
       <c r="Q13" s="2"/>
@@ -1309,7 +1319,7 @@
       </c>
       <c r="C15" s="29">
         <f t="shared" ref="C15:C21" si="1">B15/$B$22</f>
-        <v>0.10144927536231885</v>
+        <v>0.1</v>
       </c>
       <c r="D15" s="28">
         <f>B15</f>
@@ -1317,11 +1327,11 @@
       </c>
       <c r="E15" s="29">
         <f t="shared" ref="E15:E21" si="2">D15/$B$22</f>
-        <v>0.10144927536231885</v>
+        <v>0.1</v>
       </c>
       <c r="F15" s="28">
         <f>B22</f>
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="G15" s="29">
         <f t="shared" ref="G15:G21" si="3">F15/$B$22</f>
@@ -1333,15 +1343,15 @@
       </c>
       <c r="I15" s="30">
         <f t="shared" ref="I15:I21" si="5">A15-$M$17</f>
-        <v>-3.0869565217391308</v>
+        <v>-3.1285714285714281</v>
       </c>
       <c r="J15" s="30">
         <f t="shared" ref="J15:J21" si="6">B15*ABS(I15)</f>
-        <v>21.608695652173914</v>
+        <v>21.9</v>
       </c>
       <c r="K15" s="30">
         <f t="shared" ref="K15:K21" si="7">B15*(I15*I15)</f>
-        <v>66.705103969754262</v>
+        <v>68.515714285714267</v>
       </c>
       <c r="M15" s="2"/>
       <c r="P15" s="1"/>
@@ -1359,7 +1369,7 @@
       </c>
       <c r="C16" s="29">
         <f t="shared" si="1"/>
-        <v>0.13043478260869565</v>
+        <v>0.12857142857142856</v>
       </c>
       <c r="D16" s="28">
         <f t="shared" ref="D16:D21" si="8">D15+B16</f>
@@ -1367,15 +1377,15 @@
       </c>
       <c r="E16" s="29">
         <f t="shared" si="2"/>
-        <v>0.2318840579710145</v>
+        <v>0.22857142857142856</v>
       </c>
       <c r="F16" s="28">
         <f t="shared" ref="F16:F21" si="9">F15-B15</f>
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="G16" s="29">
         <f t="shared" si="3"/>
-        <v>0.89855072463768115</v>
+        <v>0.9</v>
       </c>
       <c r="H16" s="28">
         <f t="shared" si="4"/>
@@ -1383,15 +1393,15 @@
       </c>
       <c r="I16" s="30">
         <f t="shared" si="5"/>
-        <v>-2.0869565217391308</v>
+        <v>-2.1285714285714281</v>
       </c>
       <c r="J16" s="30">
         <f t="shared" si="6"/>
-        <v>18.782608695652179</v>
+        <v>19.157142857142851</v>
       </c>
       <c r="K16" s="30">
         <f t="shared" si="7"/>
-        <v>39.198487712665418</v>
+        <v>40.777346938775494</v>
       </c>
       <c r="L16" s="31" t="s">
         <v>37</v>
@@ -1414,7 +1424,7 @@
       </c>
       <c r="C17" s="29">
         <f t="shared" si="1"/>
-        <v>0.15942028985507245</v>
+        <v>0.15714285714285714</v>
       </c>
       <c r="D17" s="28">
         <f t="shared" si="8"/>
@@ -1422,15 +1432,15 @@
       </c>
       <c r="E17" s="29">
         <f t="shared" si="2"/>
-        <v>0.39130434782608697</v>
+        <v>0.38571428571428573</v>
       </c>
       <c r="F17" s="28">
         <f t="shared" si="9"/>
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="G17" s="29">
         <f t="shared" si="3"/>
-        <v>0.76811594202898548</v>
+        <v>0.77142857142857146</v>
       </c>
       <c r="H17" s="28">
         <f t="shared" si="4"/>
@@ -1438,19 +1448,19 @@
       </c>
       <c r="I17" s="30">
         <f t="shared" si="5"/>
-        <v>-1.0869565217391308</v>
+        <v>-1.1285714285714281</v>
       </c>
       <c r="J17" s="30">
         <f t="shared" si="6"/>
-        <v>11.956521739130439</v>
+        <v>12.414285714285709</v>
       </c>
       <c r="K17" s="30">
         <f t="shared" si="7"/>
-        <v>12.996219281663524</v>
+        <v>14.010408163265295</v>
       </c>
       <c r="M17" s="30">
         <f>H22/B22</f>
-        <v>8.0869565217391308</v>
+        <v>8.1285714285714281</v>
       </c>
       <c r="P17" s="1"/>
       <c r="Q17" s="2"/>
@@ -1467,7 +1477,7 @@
       </c>
       <c r="C18" s="29">
         <f t="shared" si="1"/>
-        <v>0.17391304347826086</v>
+        <v>0.17142857142857143</v>
       </c>
       <c r="D18" s="28">
         <f t="shared" si="8"/>
@@ -1475,15 +1485,15 @@
       </c>
       <c r="E18" s="29">
         <f t="shared" si="2"/>
-        <v>0.56521739130434778</v>
+        <v>0.55714285714285716</v>
       </c>
       <c r="F18" s="28">
         <f t="shared" si="9"/>
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="G18" s="29">
         <f t="shared" si="3"/>
-        <v>0.60869565217391308</v>
+        <v>0.61428571428571432</v>
       </c>
       <c r="H18" s="28">
         <f t="shared" si="4"/>
@@ -1491,15 +1501,15 @@
       </c>
       <c r="I18" s="30">
         <f t="shared" si="5"/>
-        <v>-8.6956521739130821E-2</v>
+        <v>-0.12857142857142811</v>
       </c>
       <c r="J18" s="30">
         <f t="shared" si="6"/>
-        <v>1.0434782608695699</v>
+        <v>1.5428571428571374</v>
       </c>
       <c r="K18" s="30">
         <f t="shared" si="7"/>
-        <v>9.0737240075615178E-2</v>
+        <v>0.19836734693877411</v>
       </c>
       <c r="M18" s="2"/>
       <c r="P18" s="1"/>
@@ -1521,7 +1531,7 @@
       </c>
       <c r="C19" s="29">
         <f t="shared" si="1"/>
-        <v>0.17391304347826086</v>
+        <v>0.17142857142857143</v>
       </c>
       <c r="D19" s="28">
         <f t="shared" si="8"/>
@@ -1529,15 +1539,15 @@
       </c>
       <c r="E19" s="29">
         <f t="shared" si="2"/>
-        <v>0.73913043478260865</v>
+        <v>0.72857142857142854</v>
       </c>
       <c r="F19" s="28">
         <f t="shared" si="9"/>
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="G19" s="29">
         <f t="shared" si="3"/>
-        <v>0.43478260869565216</v>
+        <v>0.44285714285714284</v>
       </c>
       <c r="H19" s="28">
         <f t="shared" si="4"/>
@@ -1545,15 +1555,15 @@
       </c>
       <c r="I19" s="30">
         <f t="shared" si="5"/>
-        <v>0.91304347826086918</v>
+        <v>0.87142857142857189</v>
       </c>
       <c r="J19" s="30">
         <f t="shared" si="6"/>
-        <v>10.95652173913043</v>
+        <v>10.457142857142863</v>
       </c>
       <c r="K19" s="30">
         <f t="shared" si="7"/>
-        <v>10.003780718336476</v>
+        <v>9.1126530612244991</v>
       </c>
       <c r="M19" s="9" t="s">
         <v>22</v>
@@ -1563,7 +1573,7 @@
       </c>
       <c r="P19" s="21">
         <f>(B22+1)/2</f>
-        <v>35</v>
+        <v>35.5</v>
       </c>
       <c r="Q19" s="2"/>
       <c r="R19" s="2"/>
@@ -1582,7 +1592,7 @@
       </c>
       <c r="C20" s="29">
         <f t="shared" si="1"/>
-        <v>0.14492753623188406</v>
+        <v>0.14285714285714285</v>
       </c>
       <c r="D20" s="28">
         <f t="shared" si="8"/>
@@ -1590,15 +1600,15 @@
       </c>
       <c r="E20" s="29">
         <f t="shared" si="2"/>
-        <v>0.88405797101449279</v>
+        <v>0.87142857142857144</v>
       </c>
       <c r="F20" s="28">
         <f t="shared" si="9"/>
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="G20" s="29">
         <f t="shared" si="3"/>
-        <v>0.2608695652173913</v>
+        <v>0.27142857142857141</v>
       </c>
       <c r="H20" s="28">
         <f t="shared" si="4"/>
@@ -1606,15 +1616,15 @@
       </c>
       <c r="I20" s="30">
         <f t="shared" si="5"/>
-        <v>1.9130434782608692</v>
+        <v>1.8714285714285719</v>
       </c>
       <c r="J20" s="30">
         <f t="shared" si="6"/>
-        <v>19.130434782608692</v>
+        <v>18.714285714285719</v>
       </c>
       <c r="K20" s="30">
         <f t="shared" si="7"/>
-        <v>36.597353497164448</v>
+        <v>35.022448979591857</v>
       </c>
       <c r="M20" s="28">
         <f>S19</f>
@@ -1635,15 +1645,15 @@
       </c>
       <c r="B21" s="28">
         <f t="shared" si="0"/>
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C21" s="29">
         <f t="shared" si="1"/>
-        <v>0.11594202898550725</v>
+        <v>0.12857142857142856</v>
       </c>
       <c r="D21" s="28">
         <f t="shared" si="8"/>
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="E21" s="29">
         <f t="shared" si="2"/>
@@ -1651,27 +1661,27 @@
       </c>
       <c r="F21" s="28">
         <f t="shared" si="9"/>
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="G21" s="29">
         <f t="shared" si="3"/>
-        <v>0.11594202898550725</v>
+        <v>0.12857142857142856</v>
       </c>
       <c r="H21" s="28">
         <f t="shared" si="4"/>
-        <v>88</v>
+        <v>99</v>
       </c>
       <c r="I21" s="30">
         <f t="shared" si="5"/>
-        <v>2.9130434782608692</v>
+        <v>2.8714285714285719</v>
       </c>
       <c r="J21" s="30">
         <f t="shared" si="6"/>
-        <v>23.304347826086953</v>
+        <v>25.842857142857149</v>
       </c>
       <c r="K21" s="30">
         <f t="shared" si="7"/>
-        <v>67.886578449905457</v>
+        <v>74.205918367346968</v>
       </c>
       <c r="M21" s="2"/>
       <c r="P21" s="1"/>
@@ -1685,11 +1695,11 @@
       </c>
       <c r="B22" s="28">
         <f>SUM(B15:B21)</f>
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="C22" s="29">
         <f>SUM(C15:C21)</f>
-        <v>0.99999999999999989</v>
+        <v>1</v>
       </c>
       <c r="D22" s="28" t="s">
         <v>39</v>
@@ -1705,18 +1715,18 @@
       </c>
       <c r="H22" s="28">
         <f>SUM(H15:H21)</f>
-        <v>558</v>
+        <v>569</v>
       </c>
       <c r="I22" s="30" t="s">
         <v>39</v>
       </c>
       <c r="J22" s="30">
         <f>SUM(J15:J21)</f>
-        <v>106.78260869565217</v>
+        <v>110.02857142857144</v>
       </c>
       <c r="K22" s="30">
         <f>SUM(K15:K21)</f>
-        <v>233.47826086956519</v>
+        <v>241.84285714285716</v>
       </c>
       <c r="M22" s="2"/>
       <c r="P22" s="1"/>
@@ -1770,7 +1780,7 @@
       </c>
       <c r="B25" s="21">
         <f>$B$22*1/4</f>
-        <v>17.25</v>
+        <v>17.5</v>
       </c>
       <c r="C25" s="2"/>
       <c r="D25" s="2"/>
@@ -1876,7 +1886,7 @@
       </c>
       <c r="B30" s="21">
         <f>$B$22*3/4</f>
-        <v>51.75</v>
+        <v>52.5</v>
       </c>
       <c r="C30" s="2"/>
       <c r="D30" s="2"/>
@@ -1978,7 +1988,7 @@
       </c>
       <c r="B35" s="23">
         <f>$B$22*6/10</f>
-        <v>41.4</v>
+        <v>42</v>
       </c>
       <c r="C35" s="23">
         <f>A19</f>
@@ -2058,7 +2068,7 @@
       </c>
       <c r="B39" s="23">
         <f>$B$22*9/10</f>
-        <v>62.1</v>
+        <v>63</v>
       </c>
       <c r="C39" s="23">
         <f>A21</f>
@@ -2125,7 +2135,7 @@
       </c>
       <c r="B42" s="21">
         <f>$B$22*27/100</f>
-        <v>18.63</v>
+        <v>18.899999999999999</v>
       </c>
       <c r="C42" s="2"/>
       <c r="D42" s="2"/>
@@ -2214,7 +2224,7 @@
       </c>
       <c r="B46" s="21">
         <f>$B$22*73/100</f>
-        <v>50.37</v>
+        <v>51.1</v>
       </c>
       <c r="C46" s="2"/>
       <c r="D46" s="2"/>
@@ -2299,7 +2309,7 @@
       </c>
       <c r="B50" s="23">
         <f>J6-J5</f>
-        <v>11106</v>
+        <v>6</v>
       </c>
       <c r="C50" s="2"/>
       <c r="D50" s="2"/>
@@ -2340,7 +2350,7 @@
       </c>
       <c r="B52" s="21">
         <f>SQRT(K22/B22)</f>
-        <v>1.8394952870701025</v>
+        <v>1.8587355807601236</v>
       </c>
       <c r="C52" s="2"/>
       <c r="D52" s="2"/>
@@ -2363,7 +2373,7 @@
       </c>
       <c r="B53" s="22">
         <f>B52*B52</f>
-        <v>3.3837429111531185</v>
+        <v>3.4548979591836737</v>
       </c>
       <c r="C53" s="2"/>
       <c r="D53" s="2"/>
@@ -2407,36 +2417,36 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="37" t="s">
+      <c r="A1" s="40" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="38"/>
-      <c r="C1" s="38"/>
-      <c r="D1" s="38"/>
-      <c r="E1" s="39"/>
-      <c r="F1" s="40"/>
-      <c r="G1" s="39"/>
-      <c r="H1" s="40"/>
-      <c r="I1" s="39"/>
-      <c r="J1" s="41"/>
+      <c r="B1" s="41"/>
+      <c r="C1" s="41"/>
+      <c r="D1" s="41"/>
+      <c r="E1" s="42"/>
+      <c r="F1" s="43"/>
+      <c r="G1" s="42"/>
+      <c r="H1" s="43"/>
+      <c r="I1" s="42"/>
+      <c r="J1" s="44"/>
       <c r="K1" s="1"/>
       <c r="L1" s="1"/>
       <c r="M1" s="1"/>
       <c r="N1" s="2"/>
     </row>
     <row r="2" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="42" t="s">
+      <c r="A2" s="45" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="43"/>
-      <c r="C2" s="43"/>
-      <c r="D2" s="43"/>
-      <c r="E2" s="44"/>
-      <c r="F2" s="45"/>
-      <c r="G2" s="44"/>
-      <c r="H2" s="45"/>
-      <c r="I2" s="44"/>
-      <c r="J2" s="46"/>
+      <c r="B2" s="46"/>
+      <c r="C2" s="46"/>
+      <c r="D2" s="46"/>
+      <c r="E2" s="47"/>
+      <c r="F2" s="48"/>
+      <c r="G2" s="47"/>
+      <c r="H2" s="48"/>
+      <c r="I2" s="47"/>
+      <c r="J2" s="49"/>
       <c r="K2" s="1"/>
       <c r="L2" s="1"/>
       <c r="M2" s="1"/>

</xml_diff>

<commit_message>
ya esta la tabla y la mayoria de datos  solo fatan los de posicion
</commit_message>
<xml_diff>
--- a/ej.xlsx
+++ b/ej.xlsx
@@ -8,13 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\proyectos del cuarto semestre\analizadorDeDatos_Estadistica\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{0F117894-3A69-4DCE-9743-6E1A83088C09}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BBDB1398-D600-45E5-A3F8-754DDDC04743}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="19440" windowHeight="14880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Hoja2" sheetId="1" r:id="rId1"/>
-    <sheet name="Hoja1" sheetId="2" r:id="rId2"/>
+    <sheet name="intervalos" sheetId="1" r:id="rId1"/>
+    <sheet name="simple" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="49">
   <si>
     <t>n</t>
   </si>
@@ -180,6 +180,18 @@
   <si>
     <t xml:space="preserve">desciavion media </t>
   </si>
+  <si>
+    <t>f*d3</t>
+  </si>
+  <si>
+    <t>f*d4</t>
+  </si>
+  <si>
+    <t>asimetria</t>
+  </si>
+  <si>
+    <t>curtosis</t>
+  </si>
 </sst>
 </file>
 
@@ -189,7 +201,7 @@
     <numFmt numFmtId="164" formatCode="#,##0.0"/>
     <numFmt numFmtId="165" formatCode="#,##0%"/>
   </numFmts>
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -227,6 +239,12 @@
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -806,10 +824,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:N68"/>
+  <dimension ref="A1:O68"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+    <sheetView tabSelected="1" topLeftCell="C31" workbookViewId="0">
+      <selection activeCell="O36" sqref="O36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -818,7 +836,8 @@
     <col min="2" max="2" width="14.5546875" style="20" bestFit="1" customWidth="1"/>
     <col min="3" max="10" width="11.5546875" style="20" bestFit="1" customWidth="1"/>
     <col min="11" max="13" width="11.5546875" style="21" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="11.5546875" style="20" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="12.109375" style="20" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="20.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -1147,8 +1166,8 @@
         <v>32</v>
       </c>
       <c r="M9" s="24">
-        <f>1+3.322*LOG(M6)</f>
-        <v>9.492036907548929</v>
+        <f>1+3.322*LOG(M5)</f>
+        <v>8.492015261953183</v>
       </c>
       <c r="N9" s="3"/>
     </row>
@@ -1189,11 +1208,11 @@
       </c>
       <c r="M10" s="24">
         <f>M8/M9</f>
-        <v>14.222447859703932</v>
+        <v>15.897286549264832</v>
       </c>
       <c r="N10" s="23">
         <f>ROUND(M10, 0)</f>
-        <v>14</v>
+        <v>16</v>
       </c>
     </row>
     <row r="11" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -1412,7 +1431,7 @@
       <c r="M16" s="1"/>
       <c r="N16" s="3"/>
     </row>
-    <row r="17" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:15" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="7">
         <v>370</v>
       </c>
@@ -1448,7 +1467,7 @@
       <c r="M17" s="1"/>
       <c r="N17" s="3"/>
     </row>
-    <row r="18" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:15" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" s="7">
         <v>371</v>
       </c>
@@ -1484,7 +1503,7 @@
       <c r="M18" s="1"/>
       <c r="N18" s="3"/>
     </row>
-    <row r="19" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:15" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A19" s="7">
         <v>372</v>
       </c>
@@ -1520,7 +1539,7 @@
       <c r="M19" s="1"/>
       <c r="N19" s="3"/>
     </row>
-    <row r="20" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:15" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A20" s="3"/>
       <c r="B20" s="1"/>
       <c r="C20" s="1"/>
@@ -1536,7 +1555,7 @@
       <c r="M20" s="1"/>
       <c r="N20" s="3"/>
     </row>
-    <row r="21" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:15" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A21" s="3"/>
       <c r="B21" s="1"/>
       <c r="C21" s="1"/>
@@ -1552,7 +1571,7 @@
       <c r="M21" s="1"/>
       <c r="N21" s="3"/>
     </row>
-    <row r="22" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:15" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A22" s="13" t="s">
         <v>34</v>
       </c>
@@ -1592,9 +1611,14 @@
       <c r="M22" s="14" t="s">
         <v>14</v>
       </c>
-      <c r="N22" s="3"/>
-    </row>
-    <row r="23" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="N22" s="14" t="s">
+        <v>45</v>
+      </c>
+      <c r="O22" s="14" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="23" spans="1:15" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A23" s="23">
         <f>M6</f>
         <v>360</v>
@@ -1636,22 +1660,29 @@
         <v>8085</v>
       </c>
       <c r="K23" s="24">
-        <f t="shared" ref="K23:K31" si="7">C23-$B$34</f>
+        <f>C23-$B$34</f>
         <v>-59.644444444444446</v>
       </c>
       <c r="L23" s="24">
-        <f t="shared" ref="L23:L31" si="8">D23*ABS(K23)</f>
+        <f t="shared" ref="L23:L31" si="7">D23*ABS(K23)</f>
         <v>1312.1777777777779</v>
       </c>
       <c r="M23" s="24">
-        <f t="shared" ref="M23:M31" si="9">D23*(K23*K23)</f>
+        <f t="shared" ref="M23:N31" si="8">D23*(K23*K23)</f>
         <v>78264.114567901241</v>
       </c>
-      <c r="N23" s="3"/>
-    </row>
-    <row r="24" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="N23" s="24">
+        <f>D23*(K23^3)</f>
+        <v>-4668019.6333388202</v>
+      </c>
+      <c r="O23" s="24">
+        <f>D23*(K23^4)</f>
+        <v>278421437.68625319</v>
+      </c>
+    </row>
+    <row r="24" spans="1:15" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A24" s="23">
-        <f t="shared" ref="A24:A31" si="10">B23+1</f>
+        <f>B23+1</f>
         <v>376</v>
       </c>
       <c r="B24" s="23">
@@ -1671,7 +1702,7 @@
         <v>0.10555555555555556</v>
       </c>
       <c r="F24" s="23">
-        <f t="shared" ref="F24:F31" si="11">F23+D24</f>
+        <f t="shared" ref="F24:F31" si="9">F23+D24</f>
         <v>41</v>
       </c>
       <c r="G24" s="25">
@@ -1679,7 +1710,7 @@
         <v>0.22777777777777777</v>
       </c>
       <c r="H24" s="23">
-        <f t="shared" ref="H24:H31" si="12">H23-D23</f>
+        <f t="shared" ref="H24:H31" si="10">H23-D23</f>
         <v>158</v>
       </c>
       <c r="I24" s="25">
@@ -1691,22 +1722,29 @@
         <v>7286.5</v>
       </c>
       <c r="K24" s="24">
+        <f t="shared" ref="K24:K31" si="11">C24-$B$34</f>
+        <v>-43.644444444444446</v>
+      </c>
+      <c r="L24" s="24">
         <f t="shared" si="7"/>
-        <v>-43.644444444444446</v>
-      </c>
-      <c r="L24" s="24">
+        <v>829.24444444444453</v>
+      </c>
+      <c r="M24" s="24">
         <f t="shared" si="8"/>
-        <v>829.24444444444453</v>
-      </c>
-      <c r="M24" s="24">
-        <f t="shared" si="9"/>
         <v>36191.91308641975</v>
       </c>
-      <c r="N24" s="3"/>
-    </row>
-    <row r="25" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="N24" s="24">
+        <f t="shared" ref="N24:O31" si="12">D24*(K24^3)</f>
+        <v>-1579575.9400384089</v>
+      </c>
+      <c r="O24" s="24">
+        <f t="shared" ref="O24:O31" si="13">D24*(K24^4)</f>
+        <v>68939714.360787436</v>
+      </c>
+    </row>
+    <row r="25" spans="1:15" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A25" s="23">
-        <f t="shared" si="10"/>
+        <f t="shared" ref="A25:A31" si="14">B24+1</f>
         <v>392</v>
       </c>
       <c r="B25" s="23">
@@ -1726,7 +1764,7 @@
         <v>0.1388888888888889</v>
       </c>
       <c r="F25" s="23">
-        <f t="shared" si="11"/>
+        <f t="shared" si="9"/>
         <v>66</v>
       </c>
       <c r="G25" s="25">
@@ -1734,7 +1772,7 @@
         <v>0.36666666666666664</v>
       </c>
       <c r="H25" s="23">
-        <f t="shared" si="12"/>
+        <f t="shared" si="10"/>
         <v>139</v>
       </c>
       <c r="I25" s="25">
@@ -1746,22 +1784,29 @@
         <v>9987.5</v>
       </c>
       <c r="K25" s="24">
+        <f t="shared" si="11"/>
+        <v>-27.644444444444446</v>
+      </c>
+      <c r="L25" s="24">
         <f t="shared" si="7"/>
-        <v>-27.644444444444446</v>
-      </c>
-      <c r="L25" s="24">
+        <v>691.11111111111109</v>
+      </c>
+      <c r="M25" s="24">
         <f t="shared" si="8"/>
-        <v>691.11111111111109</v>
-      </c>
-      <c r="M25" s="24">
-        <f t="shared" si="9"/>
         <v>19105.382716049386</v>
       </c>
-      <c r="N25" s="3"/>
-    </row>
-    <row r="26" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="N25" s="24">
+        <f t="shared" si="12"/>
+        <v>-528157.69108367641</v>
+      </c>
+      <c r="O25" s="24">
+        <f t="shared" si="13"/>
+        <v>14600625.949068744</v>
+      </c>
+    </row>
+    <row r="26" spans="1:15" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A26" s="23">
-        <f t="shared" si="10"/>
+        <f t="shared" si="14"/>
         <v>408</v>
       </c>
       <c r="B26" s="23">
@@ -1781,7 +1826,7 @@
         <v>0.1</v>
       </c>
       <c r="F26" s="23">
-        <f t="shared" si="11"/>
+        <f t="shared" si="9"/>
         <v>84</v>
       </c>
       <c r="G26" s="25">
@@ -1789,7 +1834,7 @@
         <v>0.46666666666666667</v>
       </c>
       <c r="H26" s="23">
-        <f t="shared" si="12"/>
+        <f t="shared" si="10"/>
         <v>114</v>
       </c>
       <c r="I26" s="25">
@@ -1801,22 +1846,29 @@
         <v>7479</v>
       </c>
       <c r="K26" s="24">
+        <f t="shared" si="11"/>
+        <v>-11.644444444444446</v>
+      </c>
+      <c r="L26" s="24">
         <f t="shared" si="7"/>
-        <v>-11.644444444444446</v>
-      </c>
-      <c r="L26" s="24">
+        <v>209.60000000000002</v>
+      </c>
+      <c r="M26" s="24">
         <f t="shared" si="8"/>
-        <v>209.60000000000002</v>
-      </c>
-      <c r="M26" s="24">
-        <f t="shared" si="9"/>
         <v>2440.675555555556</v>
       </c>
-      <c r="N26" s="3"/>
-    </row>
-    <row r="27" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="N26" s="24">
+        <f t="shared" si="12"/>
+        <v>-28420.310913580259</v>
+      </c>
+      <c r="O26" s="24">
+        <f t="shared" si="13"/>
+        <v>330938.73152702348</v>
+      </c>
+    </row>
+    <row r="27" spans="1:15" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A27" s="23">
-        <f t="shared" si="10"/>
+        <f t="shared" si="14"/>
         <v>424</v>
       </c>
       <c r="B27" s="23">
@@ -1836,7 +1888,7 @@
         <v>0.12777777777777777</v>
       </c>
       <c r="F27" s="26">
-        <f t="shared" si="11"/>
+        <f t="shared" si="9"/>
         <v>107</v>
       </c>
       <c r="G27" s="25">
@@ -1844,7 +1896,7 @@
         <v>0.59444444444444444</v>
       </c>
       <c r="H27" s="23">
-        <f t="shared" si="12"/>
+        <f t="shared" si="10"/>
         <v>96</v>
       </c>
       <c r="I27" s="25">
@@ -1856,22 +1908,29 @@
         <v>9924.5</v>
       </c>
       <c r="K27" s="24">
+        <f t="shared" si="11"/>
+        <v>4.3555555555555543</v>
+      </c>
+      <c r="L27" s="24">
         <f t="shared" si="7"/>
-        <v>4.3555555555555543</v>
-      </c>
-      <c r="L27" s="24">
+        <v>100.17777777777775</v>
+      </c>
+      <c r="M27" s="24">
         <f t="shared" si="8"/>
-        <v>100.17777777777775</v>
-      </c>
-      <c r="M27" s="24">
-        <f t="shared" si="9"/>
         <v>436.32987654320965</v>
       </c>
-      <c r="N27" s="3"/>
-    </row>
-    <row r="28" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="N27" s="24">
+        <f t="shared" si="12"/>
+        <v>1900.4590178326459</v>
+      </c>
+      <c r="O27" s="24">
+        <f t="shared" si="13"/>
+        <v>8277.5548332266335</v>
+      </c>
+    </row>
+    <row r="28" spans="1:15" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A28" s="23">
-        <f t="shared" si="10"/>
+        <f t="shared" si="14"/>
         <v>440</v>
       </c>
       <c r="B28" s="23">
@@ -1891,7 +1950,7 @@
         <v>0.12222222222222222</v>
       </c>
       <c r="F28" s="23">
-        <f t="shared" si="11"/>
+        <f t="shared" si="9"/>
         <v>129</v>
       </c>
       <c r="G28" s="25">
@@ -1899,7 +1958,7 @@
         <v>0.71666666666666667</v>
       </c>
       <c r="H28" s="23">
-        <f t="shared" si="12"/>
+        <f t="shared" si="10"/>
         <v>73</v>
       </c>
       <c r="I28" s="25">
@@ -1911,22 +1970,29 @@
         <v>9845</v>
       </c>
       <c r="K28" s="24">
+        <f t="shared" si="11"/>
+        <v>20.355555555555554</v>
+      </c>
+      <c r="L28" s="24">
         <f t="shared" si="7"/>
-        <v>20.355555555555554</v>
-      </c>
-      <c r="L28" s="24">
+        <v>447.82222222222219</v>
+      </c>
+      <c r="M28" s="24">
         <f t="shared" si="8"/>
-        <v>447.82222222222219</v>
-      </c>
-      <c r="M28" s="24">
-        <f t="shared" si="9"/>
         <v>9115.6701234567881</v>
       </c>
-      <c r="N28" s="3"/>
-    </row>
-    <row r="29" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="N28" s="24">
+        <f t="shared" si="12"/>
+        <v>185554.5296241426</v>
+      </c>
+      <c r="O28" s="24">
+        <f t="shared" si="13"/>
+        <v>3777065.5363492137</v>
+      </c>
+    </row>
+    <row r="29" spans="1:15" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A29" s="23">
-        <f t="shared" si="10"/>
+        <f t="shared" si="14"/>
         <v>456</v>
       </c>
       <c r="B29" s="23">
@@ -1946,7 +2012,7 @@
         <v>0.11666666666666667</v>
       </c>
       <c r="F29" s="23">
-        <f t="shared" si="11"/>
+        <f t="shared" si="9"/>
         <v>150</v>
       </c>
       <c r="G29" s="25">
@@ -1954,7 +2020,7 @@
         <v>0.83333333333333337</v>
       </c>
       <c r="H29" s="23">
-        <f t="shared" si="12"/>
+        <f t="shared" si="10"/>
         <v>51</v>
       </c>
       <c r="I29" s="25">
@@ -1966,22 +2032,29 @@
         <v>9733.5</v>
       </c>
       <c r="K29" s="24">
+        <f t="shared" si="11"/>
+        <v>36.355555555555554</v>
+      </c>
+      <c r="L29" s="24">
         <f t="shared" si="7"/>
-        <v>36.355555555555554</v>
-      </c>
-      <c r="L29" s="24">
+        <v>763.4666666666667</v>
+      </c>
+      <c r="M29" s="24">
         <f t="shared" si="8"/>
-        <v>763.4666666666667</v>
-      </c>
-      <c r="M29" s="24">
-        <f t="shared" si="9"/>
         <v>27756.254814814813</v>
       </c>
-      <c r="N29" s="3"/>
-    </row>
-    <row r="30" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="N29" s="24">
+        <f t="shared" si="12"/>
+        <v>1009094.0639341562</v>
+      </c>
+      <c r="O29" s="24">
+        <f t="shared" si="13"/>
+        <v>36686175.302139543</v>
+      </c>
+    </row>
+    <row r="30" spans="1:15" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A30" s="23">
-        <f t="shared" si="10"/>
+        <f t="shared" si="14"/>
         <v>472</v>
       </c>
       <c r="B30" s="23">
@@ -2001,7 +2074,7 @@
         <v>0.1111111111111111</v>
       </c>
       <c r="F30" s="23">
-        <f t="shared" si="11"/>
+        <f t="shared" si="9"/>
         <v>170</v>
       </c>
       <c r="G30" s="25">
@@ -2009,7 +2082,7 @@
         <v>0.94444444444444442</v>
       </c>
       <c r="H30" s="23">
-        <f t="shared" si="12"/>
+        <f t="shared" si="10"/>
         <v>30</v>
       </c>
       <c r="I30" s="25">
@@ -2021,22 +2094,29 @@
         <v>9590</v>
       </c>
       <c r="K30" s="24">
+        <f t="shared" si="11"/>
+        <v>52.355555555555554</v>
+      </c>
+      <c r="L30" s="24">
         <f t="shared" si="7"/>
-        <v>52.355555555555554</v>
-      </c>
-      <c r="L30" s="24">
+        <v>1047.1111111111111</v>
+      </c>
+      <c r="M30" s="24">
         <f t="shared" si="8"/>
-        <v>1047.1111111111111</v>
-      </c>
-      <c r="M30" s="24">
-        <f t="shared" si="9"/>
         <v>54822.083950617278</v>
       </c>
-      <c r="N30" s="3"/>
-    </row>
-    <row r="31" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="N30" s="24">
+        <f t="shared" si="12"/>
+        <v>2870240.6619478734</v>
+      </c>
+      <c r="O30" s="24">
+        <f t="shared" si="13"/>
+        <v>150273044.43442643</v>
+      </c>
+    </row>
+    <row r="31" spans="1:15" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A31" s="23">
-        <f t="shared" si="10"/>
+        <f t="shared" si="14"/>
         <v>488</v>
       </c>
       <c r="B31" s="23">
@@ -2056,7 +2136,7 @@
         <v>5.5555555555555552E-2</v>
       </c>
       <c r="F31" s="23">
-        <f t="shared" si="11"/>
+        <f t="shared" si="9"/>
         <v>180</v>
       </c>
       <c r="G31" s="25">
@@ -2064,7 +2144,7 @@
         <v>1</v>
       </c>
       <c r="H31" s="23">
-        <f t="shared" si="12"/>
+        <f t="shared" si="10"/>
         <v>10</v>
       </c>
       <c r="I31" s="25">
@@ -2076,20 +2156,27 @@
         <v>4955</v>
       </c>
       <c r="K31" s="24">
+        <f t="shared" si="11"/>
+        <v>68.355555555555554</v>
+      </c>
+      <c r="L31" s="24">
         <f t="shared" si="7"/>
-        <v>68.355555555555554</v>
-      </c>
-      <c r="L31" s="24">
+        <v>683.55555555555554</v>
+      </c>
+      <c r="M31" s="24">
         <f t="shared" si="8"/>
-        <v>683.55555555555554</v>
-      </c>
-      <c r="M31" s="24">
-        <f t="shared" si="9"/>
         <v>46724.81975308642</v>
       </c>
-      <c r="N31" s="3"/>
-    </row>
-    <row r="32" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="N31" s="24">
+        <f t="shared" si="12"/>
+        <v>3193901.0124554182</v>
+      </c>
+      <c r="O31" s="24">
+        <f t="shared" si="13"/>
+        <v>218320878.09584153</v>
+      </c>
+    </row>
+    <row r="32" spans="1:15" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A32" s="27"/>
       <c r="B32" s="22"/>
       <c r="C32" s="22"/>
@@ -2118,7 +2205,14 @@
         <f>SUM(M23:M31)</f>
         <v>274857.24444444443</v>
       </c>
-      <c r="N32" s="3"/>
+      <c r="N32" s="24">
+        <f>SUM(N23:N31)</f>
+        <v>456517.15160493786</v>
+      </c>
+      <c r="O32" s="24">
+        <f>SUM(O23:O31)</f>
+        <v>771358157.6512264</v>
+      </c>
     </row>
     <row r="33" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A33" s="3"/>
@@ -2163,7 +2257,7 @@
       </c>
       <c r="B35" s="1">
         <f>A27+((D35-F26)/D27)*N10</f>
-        <v>427.6521739130435</v>
+        <v>428.17391304347825</v>
       </c>
       <c r="C35" s="29" t="s">
         <v>18</v>
@@ -2178,8 +2272,13 @@
       <c r="H35" s="3"/>
       <c r="I35" s="4"/>
       <c r="J35" s="3"/>
-      <c r="K35" s="1"/>
-      <c r="L35" s="1"/>
+      <c r="K35" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="L35" s="1">
+        <f>N32/(D32*B65^3)</f>
+        <v>4.250427072720725E-2</v>
+      </c>
       <c r="M35" s="1"/>
       <c r="N35" s="3"/>
     </row>
@@ -2189,7 +2288,7 @@
       </c>
       <c r="B36" s="1">
         <f>A25+(D36/(D36+F36)*N10)</f>
-        <v>398.46153846153845</v>
+        <v>399.38461538461536</v>
       </c>
       <c r="C36" s="29" t="s">
         <v>39</v>
@@ -2225,8 +2324,13 @@
       <c r="H37" s="3"/>
       <c r="I37" s="4"/>
       <c r="J37" s="3"/>
-      <c r="K37" s="1"/>
-      <c r="L37" s="1"/>
+      <c r="K37" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="L37" s="1">
+        <f>O32/(D32*B65^4)</f>
+        <v>1.8378675320775366</v>
+      </c>
       <c r="M37" s="1"/>
       <c r="N37" s="3"/>
     </row>
@@ -2268,7 +2372,7 @@
       </c>
       <c r="B40" s="1">
         <f>A27+((D40-F26)/D27)*N10</f>
-        <v>427.6521739130435</v>
+        <v>428.17391304347825</v>
       </c>
       <c r="C40" s="29" t="s">
         <v>18</v>
@@ -2374,7 +2478,7 @@
       </c>
       <c r="B46" s="1">
         <f>A29+((D46-F28)/D29)*N10</f>
-        <v>466</v>
+        <v>467.42857142857144</v>
       </c>
       <c r="C46" s="29" t="s">
         <v>18</v>
@@ -2480,7 +2584,7 @@
       </c>
       <c r="B52" s="1">
         <f>A25+((D52-F24)/D25)*N10</f>
-        <v>405.32799999999997</v>
+        <v>407.23199999999997</v>
       </c>
       <c r="C52" s="29" t="s">
         <v>18</v>
@@ -2780,6 +2884,7 @@
   <mergeCells count="1">
     <mergeCell ref="A1:J1"/>
   </mergeCells>
+  <phoneticPr fontId="6" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -2791,7 +2896,9 @@
   </sheetPr>
   <dimension ref="A1:S53"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="M1" sqref="M1"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>

</xml_diff>

<commit_message>
corregi el escel a corroborando datos
</commit_message>
<xml_diff>
--- a/ej.xlsx
+++ b/ej.xlsx
@@ -1,38 +1,27 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="27830"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="27726"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\proyectos del cuarto semestre\analizadorDeDatos_Estadistica\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\tareas de la UMG\cuarto semestre\Estadistica I\analizadorDeDatos_Estadistica\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BBDB1398-D600-45E5-A3F8-754DDDC04743}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB92192C-5FFC-4DCB-A7AD-35B5FA71D77A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="19440" windowHeight="14880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="7560" yWindow="0" windowWidth="17610" windowHeight="15150" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="intervalos" sheetId="1" r:id="rId1"/>
     <sheet name="simple" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
-  <extLst>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
-  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="50">
   <si>
     <t>n</t>
   </si>
@@ -91,9 +80,6 @@
     </r>
   </si>
   <si>
-    <t xml:space="preserve"> </t>
-  </si>
-  <si>
     <t>media aritmetica</t>
   </si>
   <si>
@@ -191,6 +177,56 @@
   </si>
   <si>
     <t>curtosis</t>
+  </si>
+  <si>
+    <r>
+      <t>f*d</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>3</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t/>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>f*d</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>4</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t/>
+    </r>
   </si>
 </sst>
 </file>
@@ -826,23 +862,23 @@
   </sheetPr>
   <dimension ref="A1:O68"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C31" workbookViewId="0">
-      <selection activeCell="O36" sqref="O36"/>
+    <sheetView topLeftCell="C16" workbookViewId="0">
+      <selection activeCell="L36" sqref="L36"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="17.33203125" style="30" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.5546875" style="20" bestFit="1" customWidth="1"/>
-    <col min="3" max="10" width="11.5546875" style="20" bestFit="1" customWidth="1"/>
-    <col min="11" max="13" width="11.5546875" style="21" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="12.109375" style="20" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="20.44140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="17.28515625" style="30" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.5703125" style="20" bestFit="1" customWidth="1"/>
+    <col min="3" max="10" width="11.5703125" style="20" bestFit="1" customWidth="1"/>
+    <col min="11" max="13" width="11.5703125" style="21" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="12.140625" style="20" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="20.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="31" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B1" s="32"/>
       <c r="C1" s="32"/>
@@ -858,7 +894,7 @@
       <c r="M1" s="1"/>
       <c r="N1" s="3"/>
     </row>
-    <row r="2" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="7">
         <v>360</v>
       </c>
@@ -894,7 +930,7 @@
       <c r="M2" s="1"/>
       <c r="N2" s="3"/>
     </row>
-    <row r="3" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="7">
         <v>360</v>
       </c>
@@ -930,7 +966,7 @@
       <c r="M3" s="1"/>
       <c r="N3" s="3"/>
     </row>
-    <row r="4" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="7">
         <v>361</v>
       </c>
@@ -966,7 +1002,7 @@
       <c r="M4" s="1"/>
       <c r="N4" s="3"/>
     </row>
-    <row r="5" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="7">
         <v>361</v>
       </c>
@@ -1007,7 +1043,7 @@
       </c>
       <c r="N5" s="3"/>
     </row>
-    <row r="6" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="7">
         <v>362</v>
       </c>
@@ -1048,7 +1084,7 @@
       </c>
       <c r="N6" s="3"/>
     </row>
-    <row r="7" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="7">
         <v>363</v>
       </c>
@@ -1089,7 +1125,7 @@
       </c>
       <c r="N7" s="3"/>
     </row>
-    <row r="8" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="7">
         <v>363</v>
       </c>
@@ -1122,7 +1158,7 @@
       </c>
       <c r="K8" s="1"/>
       <c r="L8" s="22" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="M8" s="23">
         <f>M7-M6</f>
@@ -1130,7 +1166,7 @@
       </c>
       <c r="N8" s="3"/>
     </row>
-    <row r="9" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="7">
         <v>364</v>
       </c>
@@ -1163,7 +1199,7 @@
       </c>
       <c r="K9" s="1"/>
       <c r="L9" s="22" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="M9" s="24">
         <f>1+3.322*LOG(M5)</f>
@@ -1171,7 +1207,7 @@
       </c>
       <c r="N9" s="3"/>
     </row>
-    <row r="10" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="7">
         <v>364</v>
       </c>
@@ -1204,7 +1240,7 @@
       </c>
       <c r="K10" s="1"/>
       <c r="L10" s="22" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="M10" s="24">
         <f>M8/M9</f>
@@ -1215,7 +1251,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="11" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="7">
         <v>365</v>
       </c>
@@ -1251,7 +1287,7 @@
       <c r="M11" s="1"/>
       <c r="N11" s="3"/>
     </row>
-    <row r="12" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="7">
         <v>366</v>
       </c>
@@ -1287,7 +1323,7 @@
       <c r="M12" s="1"/>
       <c r="N12" s="3"/>
     </row>
-    <row r="13" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="7">
         <v>367</v>
       </c>
@@ -1323,7 +1359,7 @@
       <c r="M13" s="1"/>
       <c r="N13" s="3"/>
     </row>
-    <row r="14" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="7">
         <v>368</v>
       </c>
@@ -1359,7 +1395,7 @@
       <c r="M14" s="1"/>
       <c r="N14" s="3"/>
     </row>
-    <row r="15" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="7">
         <v>369</v>
       </c>
@@ -1395,7 +1431,7 @@
       <c r="M15" s="1"/>
       <c r="N15" s="3"/>
     </row>
-    <row r="16" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="7">
         <v>370</v>
       </c>
@@ -1431,7 +1467,7 @@
       <c r="M16" s="1"/>
       <c r="N16" s="3"/>
     </row>
-    <row r="17" spans="1:15" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:15" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="7">
         <v>370</v>
       </c>
@@ -1467,7 +1503,7 @@
       <c r="M17" s="1"/>
       <c r="N17" s="3"/>
     </row>
-    <row r="18" spans="1:15" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:15" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="7">
         <v>371</v>
       </c>
@@ -1503,7 +1539,7 @@
       <c r="M18" s="1"/>
       <c r="N18" s="3"/>
     </row>
-    <row r="19" spans="1:15" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:15" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="7">
         <v>372</v>
       </c>
@@ -1539,7 +1575,7 @@
       <c r="M19" s="1"/>
       <c r="N19" s="3"/>
     </row>
-    <row r="20" spans="1:15" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:15" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="3"/>
       <c r="B20" s="1"/>
       <c r="C20" s="1"/>
@@ -1555,7 +1591,7 @@
       <c r="M20" s="1"/>
       <c r="N20" s="3"/>
     </row>
-    <row r="21" spans="1:15" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:15" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="3"/>
       <c r="B21" s="1"/>
       <c r="C21" s="1"/>
@@ -1571,15 +1607,15 @@
       <c r="M21" s="1"/>
       <c r="N21" s="3"/>
     </row>
-    <row r="22" spans="1:15" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:15" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="13" t="s">
+        <v>33</v>
+      </c>
+      <c r="B22" s="13" t="s">
         <v>34</v>
       </c>
-      <c r="B22" s="13" t="s">
+      <c r="C22" s="13" t="s">
         <v>35</v>
-      </c>
-      <c r="C22" s="13" t="s">
-        <v>36</v>
       </c>
       <c r="D22" s="13" t="s">
         <v>5</v>
@@ -1600,7 +1636,7 @@
         <v>10</v>
       </c>
       <c r="J22" s="13" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="K22" s="14" t="s">
         <v>12</v>
@@ -1612,13 +1648,13 @@
         <v>14</v>
       </c>
       <c r="N22" s="14" t="s">
+        <v>44</v>
+      </c>
+      <c r="O22" s="14" t="s">
         <v>45</v>
       </c>
-      <c r="O22" s="14" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="23" spans="1:15" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="23" spans="1:15" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="23">
         <f>M6</f>
         <v>360</v>
@@ -1668,7 +1704,7 @@
         <v>1312.1777777777779</v>
       </c>
       <c r="M23" s="24">
-        <f t="shared" ref="M23:N31" si="8">D23*(K23*K23)</f>
+        <f t="shared" ref="M23:M31" si="8">D23*(K23*K23)</f>
         <v>78264.114567901241</v>
       </c>
       <c r="N23" s="24">
@@ -1680,7 +1716,7 @@
         <v>278421437.68625319</v>
       </c>
     </row>
-    <row r="24" spans="1:15" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:15" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="23">
         <f>B23+1</f>
         <v>376</v>
@@ -1734,7 +1770,7 @@
         <v>36191.91308641975</v>
       </c>
       <c r="N24" s="24">
-        <f t="shared" ref="N24:O31" si="12">D24*(K24^3)</f>
+        <f t="shared" ref="N24:N31" si="12">D24*(K24^3)</f>
         <v>-1579575.9400384089</v>
       </c>
       <c r="O24" s="24">
@@ -1742,7 +1778,7 @@
         <v>68939714.360787436</v>
       </c>
     </row>
-    <row r="25" spans="1:15" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:15" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="23">
         <f t="shared" ref="A25:A31" si="14">B24+1</f>
         <v>392</v>
@@ -1804,7 +1840,7 @@
         <v>14600625.949068744</v>
       </c>
     </row>
-    <row r="26" spans="1:15" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:15" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="23">
         <f t="shared" si="14"/>
         <v>408</v>
@@ -1866,7 +1902,7 @@
         <v>330938.73152702348</v>
       </c>
     </row>
-    <row r="27" spans="1:15" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:15" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="23">
         <f t="shared" si="14"/>
         <v>424</v>
@@ -1928,7 +1964,7 @@
         <v>8277.5548332266335</v>
       </c>
     </row>
-    <row r="28" spans="1:15" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:15" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="23">
         <f t="shared" si="14"/>
         <v>440</v>
@@ -1990,7 +2026,7 @@
         <v>3777065.5363492137</v>
       </c>
     </row>
-    <row r="29" spans="1:15" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:15" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="23">
         <f t="shared" si="14"/>
         <v>456</v>
@@ -2052,7 +2088,7 @@
         <v>36686175.302139543</v>
       </c>
     </row>
-    <row r="30" spans="1:15" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:15" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="23">
         <f t="shared" si="14"/>
         <v>472</v>
@@ -2114,7 +2150,7 @@
         <v>150273044.43442643</v>
       </c>
     </row>
-    <row r="31" spans="1:15" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:15" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="23">
         <f t="shared" si="14"/>
         <v>488</v>
@@ -2176,7 +2212,7 @@
         <v>218320878.09584153</v>
       </c>
     </row>
-    <row r="32" spans="1:15" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:15" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="27"/>
       <c r="B32" s="22"/>
       <c r="C32" s="22"/>
@@ -2214,7 +2250,7 @@
         <v>771358157.6512264</v>
       </c>
     </row>
-    <row r="33" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="3"/>
       <c r="B33" s="1"/>
       <c r="C33" s="1"/>
@@ -2230,9 +2266,9 @@
       <c r="M33" s="1"/>
       <c r="N33" s="3"/>
     </row>
-    <row r="34" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="29" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B34" s="1">
         <f>J32/D32</f>
@@ -2251,16 +2287,16 @@
       <c r="M34" s="1"/>
       <c r="N34" s="3"/>
     </row>
-    <row r="35" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="29" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B35" s="1">
         <f>A27+((D35-F26)/D27)*N10</f>
         <v>428.17391304347825</v>
       </c>
       <c r="C35" s="29" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D35" s="3">
         <f>D32/2</f>
@@ -2273,7 +2309,7 @@
       <c r="I35" s="4"/>
       <c r="J35" s="3"/>
       <c r="K35" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="L35" s="1">
         <f>N32/(D32*B65^3)</f>
@@ -2282,23 +2318,23 @@
       <c r="M35" s="1"/>
       <c r="N35" s="3"/>
     </row>
-    <row r="36" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="29" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B36" s="1">
         <f>A25+(D36/(D36+F36)*N10)</f>
         <v>399.38461538461536</v>
       </c>
       <c r="C36" s="29" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D36" s="3">
         <f>D25-D24</f>
         <v>6</v>
       </c>
       <c r="E36" s="29" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F36" s="3">
         <f>D25-D26</f>
@@ -2313,7 +2349,7 @@
       <c r="M36" s="1"/>
       <c r="N36" s="3"/>
     </row>
-    <row r="37" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="3"/>
       <c r="B37" s="1"/>
       <c r="C37" s="1"/>
@@ -2325,7 +2361,7 @@
       <c r="I37" s="4"/>
       <c r="J37" s="3"/>
       <c r="K37" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="L37" s="1">
         <f>O32/(D32*B65^4)</f>
@@ -2334,7 +2370,7 @@
       <c r="M37" s="1"/>
       <c r="N37" s="3"/>
     </row>
-    <row r="38" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="3"/>
       <c r="B38" s="1"/>
       <c r="C38" s="1"/>
@@ -2350,7 +2386,7 @@
       <c r="M38" s="1"/>
       <c r="N38" s="3"/>
     </row>
-    <row r="39" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="3"/>
       <c r="B39" s="1"/>
       <c r="C39" s="1"/>
@@ -2366,16 +2402,16 @@
       <c r="M39" s="1"/>
       <c r="N39" s="3"/>
     </row>
-    <row r="40" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" s="29" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B40" s="1">
         <f>A27+((D40-F26)/D27)*N10</f>
         <v>428.17391304347825</v>
       </c>
       <c r="C40" s="29" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D40" s="3">
         <f>D32*2/4</f>
@@ -2392,7 +2428,7 @@
       <c r="M40" s="1"/>
       <c r="N40" s="3"/>
     </row>
-    <row r="41" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" s="3"/>
       <c r="B41" s="1"/>
       <c r="C41" s="1"/>
@@ -2408,7 +2444,7 @@
       <c r="M41" s="1"/>
       <c r="N41" s="3"/>
     </row>
-    <row r="42" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" s="3"/>
       <c r="B42" s="1"/>
       <c r="C42" s="1"/>
@@ -2424,7 +2460,7 @@
       <c r="M42" s="1"/>
       <c r="N42" s="3"/>
     </row>
-    <row r="43" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A43" s="3"/>
       <c r="B43" s="1"/>
       <c r="C43" s="1"/>
@@ -2440,7 +2476,7 @@
       <c r="M43" s="1"/>
       <c r="N43" s="3"/>
     </row>
-    <row r="44" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A44" s="3"/>
       <c r="B44" s="1"/>
       <c r="C44" s="1"/>
@@ -2456,7 +2492,7 @@
       <c r="M44" s="1"/>
       <c r="N44" s="3"/>
     </row>
-    <row r="45" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A45" s="3"/>
       <c r="B45" s="1"/>
       <c r="C45" s="1"/>
@@ -2472,16 +2508,16 @@
       <c r="M45" s="1"/>
       <c r="N45" s="3"/>
     </row>
-    <row r="46" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A46" s="29" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B46" s="1">
         <f>A29+((D46-F28)/D29)*N10</f>
         <v>467.42857142857144</v>
       </c>
       <c r="C46" s="29" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D46" s="3">
         <f>D32*8/10</f>
@@ -2498,7 +2534,7 @@
       <c r="M46" s="1"/>
       <c r="N46" s="3"/>
     </row>
-    <row r="47" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A47" s="3"/>
       <c r="B47" s="1"/>
       <c r="C47" s="1"/>
@@ -2514,7 +2550,7 @@
       <c r="M47" s="1"/>
       <c r="N47" s="3"/>
     </row>
-    <row r="48" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A48" s="3"/>
       <c r="B48" s="1"/>
       <c r="C48" s="1"/>
@@ -2530,7 +2566,7 @@
       <c r="M48" s="1"/>
       <c r="N48" s="3"/>
     </row>
-    <row r="49" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A49" s="3"/>
       <c r="B49" s="1"/>
       <c r="C49" s="1"/>
@@ -2546,7 +2582,7 @@
       <c r="M49" s="1"/>
       <c r="N49" s="3"/>
     </row>
-    <row r="50" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A50" s="3"/>
       <c r="B50" s="1"/>
       <c r="C50" s="1"/>
@@ -2562,7 +2598,7 @@
       <c r="M50" s="1"/>
       <c r="N50" s="3"/>
     </row>
-    <row r="51" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A51" s="3"/>
       <c r="B51" s="1"/>
       <c r="C51" s="1"/>
@@ -2578,16 +2614,16 @@
       <c r="M51" s="1"/>
       <c r="N51" s="3"/>
     </row>
-    <row r="52" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A52" s="29" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B52" s="1">
         <f>A25+((D52-F24)/D25)*N10</f>
         <v>407.23199999999997</v>
       </c>
       <c r="C52" s="29" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D52" s="1">
         <f>D32*36/100</f>
@@ -2604,7 +2640,7 @@
       <c r="M52" s="1"/>
       <c r="N52" s="3"/>
     </row>
-    <row r="53" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A53" s="3"/>
       <c r="B53" s="1"/>
       <c r="C53" s="1"/>
@@ -2620,7 +2656,7 @@
       <c r="M53" s="1"/>
       <c r="N53" s="3"/>
     </row>
-    <row r="54" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A54" s="3"/>
       <c r="B54" s="1"/>
       <c r="C54" s="1"/>
@@ -2636,7 +2672,7 @@
       <c r="M54" s="1"/>
       <c r="N54" s="3"/>
     </row>
-    <row r="55" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A55" s="3"/>
       <c r="B55" s="1"/>
       <c r="C55" s="1"/>
@@ -2652,7 +2688,7 @@
       <c r="M55" s="1"/>
       <c r="N55" s="3"/>
     </row>
-    <row r="56" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A56" s="3"/>
       <c r="B56" s="1"/>
       <c r="C56" s="1"/>
@@ -2668,7 +2704,7 @@
       <c r="M56" s="1"/>
       <c r="N56" s="3"/>
     </row>
-    <row r="57" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A57" s="3"/>
       <c r="B57" s="1"/>
       <c r="C57" s="1"/>
@@ -2684,9 +2720,9 @@
       <c r="M57" s="1"/>
       <c r="N57" s="3"/>
     </row>
-    <row r="58" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A58" s="29" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B58" s="3">
         <f>M7-M6</f>
@@ -2705,7 +2741,7 @@
       <c r="M58" s="1"/>
       <c r="N58" s="3"/>
     </row>
-    <row r="59" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A59" s="3"/>
       <c r="B59" s="1"/>
       <c r="C59" s="1"/>
@@ -2721,7 +2757,7 @@
       <c r="M59" s="1"/>
       <c r="N59" s="3"/>
     </row>
-    <row r="60" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A60" s="3"/>
       <c r="B60" s="1"/>
       <c r="C60" s="1"/>
@@ -2737,7 +2773,7 @@
       <c r="M60" s="1"/>
       <c r="N60" s="3"/>
     </row>
-    <row r="61" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A61" s="3"/>
       <c r="B61" s="1"/>
       <c r="C61" s="1"/>
@@ -2753,9 +2789,9 @@
       <c r="M61" s="1"/>
       <c r="N61" s="3"/>
     </row>
-    <row r="62" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A62" s="29" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B62" s="1">
         <f>L32/D32</f>
@@ -2774,7 +2810,7 @@
       <c r="M62" s="1"/>
       <c r="N62" s="3"/>
     </row>
-    <row r="63" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A63" s="3"/>
       <c r="B63" s="1"/>
       <c r="C63" s="1"/>
@@ -2790,7 +2826,7 @@
       <c r="M63" s="1"/>
       <c r="N63" s="3"/>
     </row>
-    <row r="64" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A64" s="3"/>
       <c r="B64" s="1"/>
       <c r="C64" s="1"/>
@@ -2806,9 +2842,9 @@
       <c r="M64" s="1"/>
       <c r="N64" s="3"/>
     </row>
-    <row r="65" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A65" s="29" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B65" s="1">
         <f>SQRT(M32/D32)</f>
@@ -2827,7 +2863,7 @@
       <c r="M65" s="1"/>
       <c r="N65" s="3"/>
     </row>
-    <row r="66" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A66" s="3"/>
       <c r="B66" s="1"/>
       <c r="C66" s="1"/>
@@ -2843,7 +2879,7 @@
       <c r="M66" s="1"/>
       <c r="N66" s="3"/>
     </row>
-    <row r="67" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A67" s="3"/>
       <c r="B67" s="1"/>
       <c r="C67" s="1"/>
@@ -2859,9 +2895,9 @@
       <c r="M67" s="1"/>
       <c r="N67" s="3"/>
     </row>
-    <row r="68" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A68" s="29" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B68" s="1">
         <f>B65*B65</f>
@@ -2896,23 +2932,24 @@
   </sheetPr>
   <dimension ref="A1:S53"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="M1" sqref="M1"/>
+    <sheetView tabSelected="1" topLeftCell="E10" workbookViewId="0">
+      <selection activeCell="M25" sqref="M25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" width="11.5546875" style="19" bestFit="1" customWidth="1"/>
-    <col min="3" max="8" width="11.5546875" style="20" bestFit="1" customWidth="1"/>
-    <col min="9" max="11" width="11.5546875" style="21" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="11.5546875" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="14.6640625" style="20" bestFit="1" customWidth="1"/>
-    <col min="14" max="15" width="11.5546875" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="11.5546875" style="21" bestFit="1" customWidth="1"/>
-    <col min="17" max="19" width="11.5546875" style="20" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.5703125" style="19" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="20.28515625" style="19" customWidth="1"/>
+    <col min="3" max="8" width="11.5703125" style="20" bestFit="1" customWidth="1"/>
+    <col min="9" max="11" width="11.5703125" style="21" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="14.7109375" style="20" bestFit="1" customWidth="1"/>
+    <col min="14" max="15" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="11.5703125" style="21" bestFit="1" customWidth="1"/>
+    <col min="17" max="19" width="11.5703125" style="20" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:19" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1">
         <v>70</v>
       </c>
@@ -2932,7 +2969,7 @@
       <c r="R1" s="3"/>
       <c r="S1" s="3"/>
     </row>
-    <row r="2" spans="1:19" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:19" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="5">
         <v>11</v>
       </c>
@@ -2964,7 +3001,7 @@
       <c r="R2" s="3"/>
       <c r="S2" s="3"/>
     </row>
-    <row r="3" spans="1:19" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:19" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="7">
         <v>11</v>
       </c>
@@ -2996,7 +3033,7 @@
       <c r="R3" s="3"/>
       <c r="S3" s="3"/>
     </row>
-    <row r="4" spans="1:19" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:19" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="7">
         <v>11</v>
       </c>
@@ -3033,7 +3070,7 @@
       <c r="R4" s="3"/>
       <c r="S4" s="3"/>
     </row>
-    <row r="5" spans="1:19" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:19" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="7">
         <v>9</v>
       </c>
@@ -3070,7 +3107,7 @@
       <c r="R5" s="3"/>
       <c r="S5" s="3"/>
     </row>
-    <row r="6" spans="1:19" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:19" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="7">
         <v>8</v>
       </c>
@@ -3107,7 +3144,7 @@
       <c r="R6" s="3"/>
       <c r="S6" s="3"/>
     </row>
-    <row r="7" spans="1:19" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:19" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="7">
         <v>10</v>
       </c>
@@ -3139,7 +3176,7 @@
       <c r="R7" s="3"/>
       <c r="S7" s="3"/>
     </row>
-    <row r="8" spans="1:19" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:19" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="7">
         <v>9</v>
       </c>
@@ -3171,7 +3208,7 @@
       <c r="R8" s="3"/>
       <c r="S8" s="3"/>
     </row>
-    <row r="9" spans="1:19" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:19" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="7">
         <v>11</v>
       </c>
@@ -3203,7 +3240,7 @@
       <c r="R9" s="3"/>
       <c r="S9" s="3"/>
     </row>
-    <row r="10" spans="1:19" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:19" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="7">
         <v>6</v>
       </c>
@@ -3235,7 +3272,7 @@
       <c r="R10" s="3"/>
       <c r="S10" s="3"/>
     </row>
-    <row r="11" spans="1:19" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:19" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="7">
         <v>8</v>
       </c>
@@ -3267,7 +3304,7 @@
       <c r="R11" s="3"/>
       <c r="S11" s="3"/>
     </row>
-    <row r="12" spans="1:19" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:19" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="11"/>
       <c r="B12" s="12"/>
       <c r="C12" s="3"/>
@@ -3285,7 +3322,7 @@
       <c r="R12" s="3"/>
       <c r="S12" s="3"/>
     </row>
-    <row r="13" spans="1:19" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="13" spans="1:19" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A13" s="36" t="s">
         <v>3</v>
       </c>
@@ -3305,7 +3342,7 @@
       <c r="R13" s="3"/>
       <c r="S13" s="3"/>
     </row>
-    <row r="14" spans="1:19" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:19" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="13" t="s">
         <v>4</v>
       </c>
@@ -3339,13 +3376,18 @@
       <c r="K14" s="14" t="s">
         <v>14</v>
       </c>
-      <c r="M14" s="3"/>
+      <c r="L14" s="14" t="s">
+        <v>48</v>
+      </c>
+      <c r="M14" s="14" t="s">
+        <v>49</v>
+      </c>
       <c r="P14" s="1"/>
       <c r="Q14" s="3"/>
       <c r="R14" s="3"/>
       <c r="S14" s="3"/>
     </row>
-    <row r="15" spans="1:19" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:19" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="15">
         <v>5</v>
       </c>
@@ -3374,28 +3416,35 @@
         <v>1</v>
       </c>
       <c r="H15" s="15">
-        <f t="shared" ref="H15:H21" si="4">B15*A15</f>
+        <f t="shared" ref="H15:H16" si="4">B15*A15</f>
         <v>35</v>
       </c>
       <c r="I15" s="17">
-        <f>A15-$M$17</f>
+        <f t="shared" ref="I15:I21" si="5">A15-$K$25</f>
         <v>-3.1285714285714281</v>
       </c>
       <c r="J15" s="17">
-        <f t="shared" ref="J15:J21" si="5">B15*ABS(I15)</f>
+        <f t="shared" ref="J15:J21" si="6">B15*ABS(I15)</f>
         <v>21.9</v>
       </c>
       <c r="K15" s="17">
-        <f t="shared" ref="K15:K21" si="6">B15*(I15*I15)</f>
+        <f>B15*(I15*I15)</f>
         <v>68.515714285714267</v>
       </c>
-      <c r="M15" s="3"/>
+      <c r="L15" s="17">
+        <f>B15*I15^3</f>
+        <v>-214.35630612244887</v>
+      </c>
+      <c r="M15" s="17">
+        <f>B15*I15^4</f>
+        <v>670.62901486880423</v>
+      </c>
       <c r="P15" s="1"/>
       <c r="Q15" s="3"/>
       <c r="R15" s="3"/>
       <c r="S15" s="3"/>
     </row>
-    <row r="16" spans="1:19" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:19" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="15">
         <v>6</v>
       </c>
@@ -3428,29 +3477,27 @@
         <v>54</v>
       </c>
       <c r="I16" s="17">
-        <f>A16-$M$17</f>
+        <f t="shared" si="5"/>
         <v>-2.1285714285714281</v>
       </c>
       <c r="J16" s="17">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>19.157142857142851</v>
       </c>
       <c r="K16" s="17">
-        <f t="shared" si="6"/>
+        <f t="shared" ref="K16:K21" si="9">B16*(I16*I16)</f>
         <v>40.777346938775494</v>
       </c>
-      <c r="L16" s="18" t="s">
-        <v>15</v>
-      </c>
-      <c r="M16" s="13" t="s">
-        <v>16</v>
-      </c>
-      <c r="P16" s="1"/>
-      <c r="Q16" s="3"/>
-      <c r="R16" s="3"/>
-      <c r="S16" s="3"/>
-    </row>
-    <row r="17" spans="1:19" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="L16" s="17">
+        <f t="shared" ref="L16:L21" si="10">B16*I16^3</f>
+        <v>-86.797495626822098</v>
+      </c>
+      <c r="M16" s="17">
+        <f t="shared" ref="M16:M21" si="11">B16*I16^4</f>
+        <v>184.754669262807</v>
+      </c>
+    </row>
+    <row r="17" spans="1:19" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="15">
         <v>7</v>
       </c>
@@ -3479,31 +3526,31 @@
         <v>0.77142857142857146</v>
       </c>
       <c r="H17" s="15">
-        <f t="shared" si="4"/>
+        <f>B17*A17</f>
         <v>77</v>
       </c>
       <c r="I17" s="17">
-        <f>A17-$M$17</f>
+        <f t="shared" si="5"/>
         <v>-1.1285714285714281</v>
       </c>
       <c r="J17" s="17">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>12.414285714285709</v>
       </c>
       <c r="K17" s="17">
-        <f t="shared" si="6"/>
+        <f t="shared" si="9"/>
         <v>14.010408163265295</v>
       </c>
+      <c r="L17" s="17">
+        <f t="shared" si="10"/>
+        <v>-15.811746355685113</v>
+      </c>
       <c r="M17" s="17">
-        <f>H22/B22</f>
-        <v>8.1285714285714281</v>
-      </c>
-      <c r="P17" s="1"/>
-      <c r="Q17" s="3"/>
-      <c r="R17" s="3"/>
-      <c r="S17" s="3"/>
-    </row>
-    <row r="18" spans="1:19" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+        <f t="shared" si="11"/>
+        <v>17.844685172844621</v>
+      </c>
+    </row>
+    <row r="18" spans="1:19" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="15">
         <v>8</v>
       </c>
@@ -3532,32 +3579,31 @@
         <v>0.61428571428571432</v>
       </c>
       <c r="H18" s="15">
-        <f t="shared" si="4"/>
+        <f>B18*A18</f>
         <v>96</v>
       </c>
       <c r="I18" s="17">
-        <f>A20-$M$17</f>
-        <v>1.8714285714285719</v>
+        <f t="shared" si="5"/>
+        <v>-0.12857142857142811</v>
       </c>
       <c r="J18" s="17">
-        <f t="shared" si="5"/>
-        <v>22.457142857142863</v>
+        <f t="shared" si="6"/>
+        <v>1.5428571428571374</v>
       </c>
       <c r="K18" s="17">
-        <f t="shared" si="6"/>
-        <v>42.026938775510224</v>
-      </c>
-      <c r="M18" s="3"/>
-      <c r="P18" s="1"/>
-      <c r="Q18" s="10">
-        <v>35</v>
-      </c>
-      <c r="R18" s="10">
-        <v>8</v>
-      </c>
-      <c r="S18" s="3"/>
-    </row>
-    <row r="19" spans="1:19" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+        <f t="shared" si="9"/>
+        <v>0.19836734693877411</v>
+      </c>
+      <c r="L18" s="17">
+        <f t="shared" si="10"/>
+        <v>-2.5504373177842293E-2</v>
+      </c>
+      <c r="M18" s="17">
+        <f t="shared" si="11"/>
+        <v>3.2791336942939973E-3</v>
+      </c>
+    </row>
+    <row r="19" spans="1:19" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="15">
         <v>9</v>
       </c>
@@ -3586,39 +3632,31 @@
         <v>0.44285714285714284</v>
       </c>
       <c r="H19" s="15">
-        <f t="shared" si="4"/>
+        <f>B19*A19</f>
         <v>108</v>
       </c>
       <c r="I19" s="17">
-        <f>A21-$M$17</f>
-        <v>2.8714285714285719</v>
+        <f t="shared" si="5"/>
+        <v>0.87142857142857189</v>
       </c>
       <c r="J19" s="17">
-        <f t="shared" si="5"/>
-        <v>34.457142857142863</v>
+        <f t="shared" si="6"/>
+        <v>10.457142857142863</v>
       </c>
       <c r="K19" s="17">
-        <f t="shared" si="6"/>
-        <v>98.941224489795957</v>
-      </c>
-      <c r="M19" s="13" t="s">
-        <v>17</v>
-      </c>
-      <c r="O19" s="18" t="s">
-        <v>18</v>
-      </c>
-      <c r="P19" s="9">
-        <f>(B22+1)/2</f>
-        <v>35.5</v>
-      </c>
-      <c r="Q19" s="3"/>
-      <c r="R19" s="3"/>
-      <c r="S19" s="10">
-        <f>AVERAGE(R18:R20)</f>
-        <v>8</v>
-      </c>
-    </row>
-    <row r="20" spans="1:19" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+        <f t="shared" si="9"/>
+        <v>9.1126530612244991</v>
+      </c>
+      <c r="L19" s="17">
+        <f t="shared" si="10"/>
+        <v>7.9410262390670674</v>
+      </c>
+      <c r="M19" s="17">
+        <f t="shared" si="11"/>
+        <v>6.92003715118702</v>
+      </c>
+    </row>
+    <row r="20" spans="1:19" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="15">
         <v>10</v>
       </c>
@@ -3647,35 +3685,31 @@
         <v>0.27142857142857141</v>
       </c>
       <c r="H20" s="15">
-        <f t="shared" si="4"/>
+        <f>B20*A20</f>
         <v>100</v>
       </c>
-      <c r="I20" s="17" t="e">
-        <f>A22-$M$17</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="J20" s="17" t="e">
+      <c r="I20" s="17">
         <f t="shared" si="5"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="K20" s="17" t="e">
+        <v>1.8714285714285719</v>
+      </c>
+      <c r="J20" s="17">
         <f t="shared" si="6"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="M20" s="15">
-        <f>S19</f>
-        <v>8</v>
-      </c>
-      <c r="P20" s="1"/>
-      <c r="Q20" s="10">
-        <v>36</v>
-      </c>
-      <c r="R20" s="10">
-        <v>8</v>
-      </c>
-      <c r="S20" s="3"/>
-    </row>
-    <row r="21" spans="1:19" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+        <v>18.714285714285719</v>
+      </c>
+      <c r="K20" s="17">
+        <f>B20*(I20*I20)</f>
+        <v>35.022448979591857</v>
+      </c>
+      <c r="L20" s="17">
+        <f t="shared" si="10"/>
+        <v>65.542011661807621</v>
+      </c>
+      <c r="M20" s="17">
+        <f t="shared" si="11"/>
+        <v>122.65719325281145</v>
+      </c>
+    </row>
+    <row r="21" spans="1:19" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="15">
         <v>11</v>
       </c>
@@ -3704,30 +3738,37 @@
         <v>0.12857142857142856</v>
       </c>
       <c r="H21" s="15">
-        <f t="shared" si="4"/>
+        <f>B21*A21</f>
         <v>99</v>
       </c>
       <c r="I21" s="17">
-        <f>A23-$M$17</f>
-        <v>-8.1285714285714281</v>
+        <f t="shared" si="5"/>
+        <v>2.8714285714285719</v>
       </c>
       <c r="J21" s="17">
-        <f t="shared" si="5"/>
-        <v>73.157142857142858</v>
+        <f t="shared" si="6"/>
+        <v>25.842857142857149</v>
       </c>
       <c r="K21" s="17">
-        <f t="shared" si="6"/>
-        <v>594.66306122448964</v>
-      </c>
-      <c r="M21" s="3"/>
+        <f t="shared" si="9"/>
+        <v>74.205918367346968</v>
+      </c>
+      <c r="L21" s="17">
+        <f t="shared" si="10"/>
+        <v>213.07699416909634</v>
+      </c>
+      <c r="M21" s="17">
+        <f t="shared" si="11"/>
+        <v>611.83536897126237</v>
+      </c>
       <c r="P21" s="1"/>
       <c r="Q21" s="3"/>
       <c r="R21" s="3"/>
       <c r="S21" s="3"/>
     </row>
-    <row r="22" spans="1:19" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:19" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="15" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B22" s="15">
         <f>SUM(B15:B21)</f>
@@ -3738,39 +3779,46 @@
         <v>1</v>
       </c>
       <c r="D22" s="15" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E22" s="15" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F22" s="15" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="G22" s="15" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="H22" s="15">
         <f>SUM(H15:H21)</f>
         <v>569</v>
       </c>
       <c r="I22" s="17" t="s">
-        <v>20</v>
-      </c>
-      <c r="J22" s="17" t="e">
+        <v>19</v>
+      </c>
+      <c r="J22" s="17">
         <f>SUM(J15:J21)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="K22" s="17" t="e">
+        <v>110.02857142857144</v>
+      </c>
+      <c r="K22" s="17">
         <f>SUM(K15:K21)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="M22" s="3"/>
+        <v>241.84285714285716</v>
+      </c>
+      <c r="L22" s="17">
+        <f>SUM(L15:L21)</f>
+        <v>-30.431020408162908</v>
+      </c>
+      <c r="M22" s="17">
+        <f>SUM(M15:M21)</f>
+        <v>1614.6442478134109</v>
+      </c>
       <c r="P22" s="1"/>
       <c r="Q22" s="3"/>
       <c r="R22" s="3"/>
       <c r="S22" s="3"/>
     </row>
-    <row r="23" spans="1:19" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:19" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="10"/>
       <c r="B23" s="12"/>
       <c r="C23" s="3"/>
@@ -3788,7 +3836,7 @@
       <c r="R23" s="3"/>
       <c r="S23" s="3"/>
     </row>
-    <row r="24" spans="1:19" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:19" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="10"/>
       <c r="B24" s="12"/>
       <c r="C24" s="10">
@@ -3800,19 +3848,28 @@
       <c r="E24" s="1"/>
       <c r="F24" s="3"/>
       <c r="G24" s="4"/>
-      <c r="H24" s="3"/>
-      <c r="I24" s="1"/>
+      <c r="H24" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="I24" s="1">
+        <f>L22/(B22*B52^3)</f>
+        <v>-6.7696409931673404E-2</v>
+      </c>
       <c r="J24" s="1"/>
-      <c r="K24" s="1"/>
-      <c r="M24" s="3"/>
-      <c r="P24" s="1"/>
+      <c r="K24" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="M24"/>
+      <c r="N24" s="1"/>
+      <c r="O24" s="3"/>
+      <c r="P24" s="3"/>
       <c r="Q24" s="3"/>
       <c r="R24" s="3"/>
       <c r="S24" s="3"/>
     </row>
-    <row r="25" spans="1:19" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:19" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="10" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B25" s="9">
         <f>$B$22*1/4</f>
@@ -3825,17 +3882,22 @@
       </c>
       <c r="F25" s="3"/>
       <c r="G25" s="4"/>
-      <c r="H25" s="3"/>
+      <c r="H25" s="1"/>
       <c r="I25" s="1"/>
       <c r="J25" s="1"/>
-      <c r="K25" s="1"/>
-      <c r="M25" s="3"/>
-      <c r="P25" s="1"/>
+      <c r="K25" s="17">
+        <f>H22/B22</f>
+        <v>8.1285714285714281</v>
+      </c>
+      <c r="M25"/>
+      <c r="N25" s="1"/>
+      <c r="O25" s="3"/>
+      <c r="P25" s="3"/>
       <c r="Q25" s="3"/>
       <c r="R25" s="3"/>
       <c r="S25" s="3"/>
     </row>
-    <row r="26" spans="1:19" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:19" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="10"/>
       <c r="B26" s="12"/>
       <c r="C26" s="10">
@@ -3847,17 +3909,28 @@
       <c r="E26" s="1"/>
       <c r="F26" s="3"/>
       <c r="G26" s="4"/>
-      <c r="H26" s="3"/>
-      <c r="I26" s="1"/>
+      <c r="H26" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="I26" s="1">
+        <f>M22/(B22*B52^4)</f>
+        <v>1.9324504180854689</v>
+      </c>
       <c r="J26" s="1"/>
-      <c r="K26" s="1"/>
-      <c r="M26" s="3"/>
-      <c r="P26" s="1"/>
+      <c r="K26" s="3"/>
+      <c r="M26"/>
+      <c r="N26" s="1"/>
+      <c r="O26" s="10">
+        <v>35</v>
+      </c>
+      <c r="P26" s="10">
+        <v>8</v>
+      </c>
       <c r="Q26" s="3"/>
       <c r="R26" s="3"/>
       <c r="S26" s="3"/>
     </row>
-    <row r="27" spans="1:19" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:19" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="10"/>
       <c r="B27" s="12"/>
       <c r="C27" s="3"/>
@@ -3868,14 +3941,26 @@
       <c r="H27" s="3"/>
       <c r="I27" s="1"/>
       <c r="J27" s="1"/>
-      <c r="K27" s="1"/>
-      <c r="M27" s="3"/>
-      <c r="P27" s="1"/>
-      <c r="Q27" s="3"/>
+      <c r="K27" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="M27" s="18" t="s">
+        <v>17</v>
+      </c>
+      <c r="N27" s="9">
+        <f>(B22+1)/2</f>
+        <v>35.5</v>
+      </c>
+      <c r="O27" s="3"/>
+      <c r="P27" s="3"/>
+      <c r="Q27" s="10">
+        <f>AVERAGE(P26:P28)</f>
+        <v>8</v>
+      </c>
       <c r="R27" s="3"/>
       <c r="S27" s="3"/>
     </row>
-    <row r="28" spans="1:19" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:19" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="10"/>
       <c r="B28" s="12"/>
       <c r="C28" s="3"/>
@@ -3886,14 +3971,23 @@
       <c r="H28" s="3"/>
       <c r="I28" s="1"/>
       <c r="J28" s="1"/>
-      <c r="K28" s="1"/>
-      <c r="M28" s="3"/>
-      <c r="P28" s="1"/>
+      <c r="K28" s="15">
+        <f>Q27</f>
+        <v>8</v>
+      </c>
+      <c r="M28"/>
+      <c r="N28" s="1"/>
+      <c r="O28" s="10">
+        <v>36</v>
+      </c>
+      <c r="P28" s="10">
+        <v>8</v>
+      </c>
       <c r="Q28" s="3"/>
       <c r="R28" s="3"/>
       <c r="S28" s="3"/>
     </row>
-    <row r="29" spans="1:19" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:19" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="10"/>
       <c r="B29" s="12"/>
       <c r="C29" s="10">
@@ -3916,9 +4010,9 @@
       <c r="R29" s="3"/>
       <c r="S29" s="3"/>
     </row>
-    <row r="30" spans="1:19" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:19" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="10" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B30" s="9">
         <f>$B$22*3/4</f>
@@ -3942,7 +4036,7 @@
       <c r="R30" s="3"/>
       <c r="S30" s="3"/>
     </row>
-    <row r="31" spans="1:19" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:19" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="10"/>
       <c r="B31" s="12"/>
       <c r="C31" s="10">
@@ -3964,7 +4058,7 @@
       <c r="R31" s="3"/>
       <c r="S31" s="3"/>
     </row>
-    <row r="32" spans="1:19" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:19" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="10"/>
       <c r="B32" s="12"/>
       <c r="C32" s="3"/>
@@ -3982,7 +4076,7 @@
       <c r="R32" s="3"/>
       <c r="S32" s="3"/>
     </row>
-    <row r="33" spans="1:19" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:19" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="10"/>
       <c r="B33" s="12"/>
       <c r="C33" s="3"/>
@@ -4000,7 +4094,7 @@
       <c r="R33" s="3"/>
       <c r="S33" s="3"/>
     </row>
-    <row r="34" spans="1:19" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:19" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="10"/>
       <c r="B34" s="12"/>
       <c r="C34" s="3"/>
@@ -4018,9 +4112,9 @@
       <c r="R34" s="3"/>
       <c r="S34" s="3"/>
     </row>
-    <row r="35" spans="1:19" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:19" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="10" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B35" s="10">
         <f>$B$22*6/10</f>
@@ -4044,7 +4138,7 @@
       <c r="R35" s="3"/>
       <c r="S35" s="3"/>
     </row>
-    <row r="36" spans="1:19" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:19" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="10"/>
       <c r="B36" s="12"/>
       <c r="C36" s="3"/>
@@ -4062,7 +4156,7 @@
       <c r="R36" s="3"/>
       <c r="S36" s="3"/>
     </row>
-    <row r="37" spans="1:19" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:19" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="10"/>
       <c r="B37" s="12"/>
       <c r="C37" s="3"/>
@@ -4080,7 +4174,7 @@
       <c r="R37" s="3"/>
       <c r="S37" s="3"/>
     </row>
-    <row r="38" spans="1:19" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:19" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="10"/>
       <c r="B38" s="12"/>
       <c r="C38" s="3"/>
@@ -4098,9 +4192,9 @@
       <c r="R38" s="3"/>
       <c r="S38" s="3"/>
     </row>
-    <row r="39" spans="1:19" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:19" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="10" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B39" s="10">
         <f>$B$22*9/10</f>
@@ -4124,7 +4218,7 @@
       <c r="R39" s="3"/>
       <c r="S39" s="3"/>
     </row>
-    <row r="40" spans="1:19" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:19" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" s="10"/>
       <c r="B40" s="12"/>
       <c r="C40" s="3"/>
@@ -4142,7 +4236,7 @@
       <c r="R40" s="3"/>
       <c r="S40" s="3"/>
     </row>
-    <row r="41" spans="1:19" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:19" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" s="10"/>
       <c r="B41" s="12"/>
       <c r="C41" s="10">
@@ -4165,9 +4259,9 @@
       <c r="R41" s="3"/>
       <c r="S41" s="3"/>
     </row>
-    <row r="42" spans="1:19" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:19" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" s="10" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B42" s="9">
         <f>$B$22*27/100</f>
@@ -4190,7 +4284,7 @@
       <c r="R42" s="3"/>
       <c r="S42" s="3"/>
     </row>
-    <row r="43" spans="1:19" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:19" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A43" s="10"/>
       <c r="B43" s="12"/>
       <c r="C43" s="10">
@@ -4213,7 +4307,7 @@
       <c r="R43" s="3"/>
       <c r="S43" s="3"/>
     </row>
-    <row r="44" spans="1:19" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:19" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A44" s="10"/>
       <c r="B44" s="12"/>
       <c r="C44" s="3"/>
@@ -4231,7 +4325,7 @@
       <c r="R44" s="3"/>
       <c r="S44" s="3"/>
     </row>
-    <row r="45" spans="1:19" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:19" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A45" s="10"/>
       <c r="B45" s="12"/>
       <c r="C45" s="10">
@@ -4254,9 +4348,9 @@
       <c r="R45" s="3"/>
       <c r="S45" s="3"/>
     </row>
-    <row r="46" spans="1:19" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:19" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A46" s="10" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B46" s="9">
         <f>$B$22*73/100</f>
@@ -4280,7 +4374,7 @@
       <c r="R46" s="3"/>
       <c r="S46" s="3"/>
     </row>
-    <row r="47" spans="1:19" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:19" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A47" s="10"/>
       <c r="B47" s="12"/>
       <c r="C47" s="10">
@@ -4303,7 +4397,7 @@
       <c r="R47" s="3"/>
       <c r="S47" s="3"/>
     </row>
-    <row r="48" spans="1:19" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:19" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A48" s="10"/>
       <c r="B48" s="12"/>
       <c r="C48" s="3"/>
@@ -4321,7 +4415,7 @@
       <c r="R48" s="3"/>
       <c r="S48" s="3"/>
     </row>
-    <row r="49" spans="1:19" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:19" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A49" s="10"/>
       <c r="B49" s="12"/>
       <c r="C49" s="3"/>
@@ -4339,9 +4433,9 @@
       <c r="R49" s="3"/>
       <c r="S49" s="3"/>
     </row>
-    <row r="50" spans="1:19" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:19" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A50" s="10" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B50" s="10">
         <f>J6-J5</f>
@@ -4362,7 +4456,7 @@
       <c r="R50" s="3"/>
       <c r="S50" s="3"/>
     </row>
-    <row r="51" spans="1:19" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:19" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A51" s="10"/>
       <c r="B51" s="12"/>
       <c r="C51" s="3"/>
@@ -4380,13 +4474,13 @@
       <c r="R51" s="3"/>
       <c r="S51" s="3"/>
     </row>
-    <row r="52" spans="1:19" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:19" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A52" s="10" t="s">
-        <v>28</v>
-      </c>
-      <c r="B52" s="9" t="e">
+        <v>27</v>
+      </c>
+      <c r="B52" s="9">
         <f>SQRT(K22/B22)</f>
-        <v>#VALUE!</v>
+        <v>1.8587355807601236</v>
       </c>
       <c r="C52" s="3"/>
       <c r="D52" s="3"/>
@@ -4403,13 +4497,13 @@
       <c r="R52" s="3"/>
       <c r="S52" s="3"/>
     </row>
-    <row r="53" spans="1:19" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:19" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A53" s="10" t="s">
-        <v>29</v>
-      </c>
-      <c r="B53" s="12" t="e">
+        <v>28</v>
+      </c>
+      <c r="B53" s="12">
         <f>B52*B52</f>
-        <v>#VALUE!</v>
+        <v>3.4548979591836737</v>
       </c>
       <c r="C53" s="3"/>
       <c r="D53" s="3"/>
@@ -4430,6 +4524,7 @@
   <mergeCells count="1">
     <mergeCell ref="A13:K13"/>
   </mergeCells>
+  <phoneticPr fontId="6" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>